<commit_message>
Review points by EA on CRS
</commit_message>
<xml_diff>
--- a/Input Document/CRS/Review/PO_SP_CRS_MobileApplication_Review_Template.xlsx
+++ b/Input Document/CRS/Review/PO_SP_CRS_MobileApplication_Review_Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nourh\OneDrive\Desktop\Mobile_SWProcess_Documents\Mobile_SWProcess_Documents\Input Document\CRS\Review\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BB90D15-68F1-4AEC-942D-D5A647014D0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59388D3E-6B2F-4AF2-8B62-2FF6702A4530}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="89">
   <si>
     <t>Entry Date</t>
   </si>
@@ -146,6 +146,147 @@
   </si>
   <si>
     <t>page 5</t>
+  </si>
+  <si>
+    <t>CRS_REV_009</t>
+  </si>
+  <si>
+    <t>CRS_REV_010</t>
+  </si>
+  <si>
+    <t>CRS_REV_011</t>
+  </si>
+  <si>
+    <t>CRS_REV_012</t>
+  </si>
+  <si>
+    <t>CRS_REV_013</t>
+  </si>
+  <si>
+    <t>CRS_REV_014</t>
+  </si>
+  <si>
+    <t>CRS_REV_015</t>
+  </si>
+  <si>
+    <t>CRS_REV_016</t>
+  </si>
+  <si>
+    <t>CRS_REV_017</t>
+  </si>
+  <si>
+    <t>CRS_REV_018</t>
+  </si>
+  <si>
+    <t>CRS_REV_019</t>
+  </si>
+  <si>
+    <t>CRS_REV_020</t>
+  </si>
+  <si>
+    <t>CRS_REV_021</t>
+  </si>
+  <si>
+    <t>CRS_REV_022</t>
+  </si>
+  <si>
+    <t>page 6</t>
+  </si>
+  <si>
+    <t>page 7</t>
+  </si>
+  <si>
+    <t>page 8</t>
+  </si>
+  <si>
+    <t>CRS_REV_023</t>
+  </si>
+  <si>
+    <t>CRS_REV_024</t>
+  </si>
+  <si>
+    <t>CRS_REV_025</t>
+  </si>
+  <si>
+    <t>CRS_REV_026</t>
+  </si>
+  <si>
+    <t>CRS_REV_027</t>
+  </si>
+  <si>
+    <t>CRS_REV_028</t>
+  </si>
+  <si>
+    <t>CRS_REV_029</t>
+  </si>
+  <si>
+    <t>CRS_REV_030</t>
+  </si>
+  <si>
+    <t>CRS_REV_031</t>
+  </si>
+  <si>
+    <t>Esraa Abdelnaby</t>
+  </si>
+  <si>
+    <t>edit the context diagram</t>
+  </si>
+  <si>
+    <t>add requirments based on the change request of the CR</t>
+  </si>
+  <si>
+    <t>Allow sign up with "Gmail" &amp; "Fcebook"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">add reset password option </t>
+  </si>
+  <si>
+    <t>Verify the accuracy of the information while logging in</t>
+  </si>
+  <si>
+    <t>Prevent the duplication of email during registration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">app shall let users choose the plan </t>
+  </si>
+  <si>
+    <t>The ride starts after the current location is determined</t>
+  </si>
+  <si>
+    <t>The app shall automatically detect the current location if it has access to the location</t>
+  </si>
+  <si>
+    <t xml:space="preserve">app shall allow reporting of any issue </t>
+  </si>
+  <si>
+    <t xml:space="preserve">users of basic plan can upgrade to premium plan </t>
+  </si>
+  <si>
+    <t xml:space="preserve">on basic plan , the icons of all saved bumbs appear on the gps screen </t>
+  </si>
+  <si>
+    <t xml:space="preserve">voice notify users with the recorded speed bumbs </t>
+  </si>
+  <si>
+    <t>at choosing premium plan , app shall redirect the user to the website</t>
+  </si>
+  <si>
+    <t>on premium plan ,any upcoming bump shall appear on the screen</t>
+  </si>
+  <si>
+    <t>The app notifies the user of the time left until the next bump</t>
+  </si>
+  <si>
+    <t>by the end of the ride ,the app shall save the detected bumps</t>
+  </si>
+  <si>
+    <t>The user has to give the permission to connect to the detecting device via bluetooth</t>
+  </si>
+  <si>
+    <t>page 4</t>
+  </si>
+  <si>
+    <t>V1.2</t>
   </si>
 </sst>
 </file>
@@ -498,10 +639,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -748,21 +889,523 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:8" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10" s="3">
+        <v>44892</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="G10" s="5"/>
+      <c r="H10" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11" s="3">
+        <v>44892</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="G11" s="5"/>
+      <c r="H11" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B12" s="3">
+        <v>44892</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="G12" s="5"/>
+      <c r="H12" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13" s="3">
+        <v>44892</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="G13" s="5"/>
+      <c r="H13" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B14" s="3">
+        <v>44892</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="G14" s="5"/>
+      <c r="H14" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B15" s="3">
+        <v>44892</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="G15" s="5"/>
+      <c r="H15" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B16" s="3">
+        <v>44892</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="G16" s="5"/>
+      <c r="H16" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B17" s="3">
+        <v>44892</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="G17" s="5"/>
+      <c r="H17" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B18" s="3">
+        <v>44892</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="G18" s="5"/>
+      <c r="H18" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B19" s="3">
+        <v>44892</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="G19" s="5"/>
+      <c r="H19" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B20" s="3">
+        <v>44892</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="G20" s="5"/>
+      <c r="H20" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B21" s="3">
+        <v>44892</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="G21" s="5"/>
+      <c r="H21" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B22" s="3">
+        <v>44892</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="G22" s="5"/>
+      <c r="H22" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B23" s="3">
+        <v>44892</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="G23" s="5"/>
+      <c r="H23" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B24" s="3">
+        <v>44892</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="G24" s="5"/>
+      <c r="H24" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B25" s="3">
+        <v>44892</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="G25" s="5"/>
+      <c r="H25" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B26" s="3">
+        <v>44893</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="G26" s="5"/>
+      <c r="H26" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B27" s="3">
+        <v>44894</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="G27" s="5"/>
+      <c r="H27" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B28" s="3"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="5"/>
+      <c r="H28" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B29" s="3"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="5"/>
+      <c r="H29" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B30" s="3"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="5"/>
+      <c r="G30" s="5"/>
+      <c r="H30" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B31" s="3"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="5"/>
+      <c r="G31" s="5"/>
+      <c r="H31" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B32" s="3"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="5"/>
+      <c r="H32" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
-  <conditionalFormatting sqref="A2:H9">
+  <conditionalFormatting sqref="A2:H32">
     <cfRule type="expression" dxfId="1" priority="3">
       <formula>$H2 = "Closed"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:H9">
+  <conditionalFormatting sqref="A2:H32">
     <cfRule type="expression" dxfId="0" priority="4">
       <formula>$H2= "Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Open" sqref="H2:H9" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Open" sqref="H2:H32" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Open,Closed"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>